<commit_message>
BOM.xlsx -- added highlighting to make it clear which is the total and which is a per board price.
Per Saleem's suggestion changed the 5V_IN line to be 25 mils
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13110"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -12,17 +12,18 @@
     <sheet name="Calc" sheetId="5" r:id="rId3"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Calc!$A$1:$K$12</definedName>
     <definedName name="BOM">BOM!$A$1:$L$39</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="25" r:id="rId4"/>
+    <pivotCache cacheId="3" r:id="rId4"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="260" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="90">
   <si>
     <t>#</t>
   </si>
@@ -291,6 +292,18 @@
   </si>
   <si>
     <t>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</t>
+  </si>
+  <si>
+    <t>SMD</t>
+  </si>
+  <si>
+    <t>SMD only</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Per Board</t>
   </si>
 </sst>
 </file>
@@ -823,7 +836,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -838,6 +851,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" xfId="13"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -895,7 +910,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Nick Rapoport" refreshedDate="42439.135842129632" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="38">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Nick Rapoport" refreshedDate="42440.935864120373" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="38">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:L39" sheet="BOM"/>
   </cacheSource>
@@ -1501,7 +1516,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="25" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -1896,8 +1911,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E34" sqref="E34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1987,7 +2002,7 @@
         <v>32</v>
       </c>
       <c r="L2" t="str">
-        <f>CONCATENATE(K2," DigiKey Part: ",H2," (",E2,")")</f>
+        <f t="shared" ref="L2:L33" si="0">CONCATENATE(K2," DigiKey Part: ",H2," (",E2,")")</f>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -2026,7 +2041,7 @@
         <v>32</v>
       </c>
       <c r="L3" t="str">
-        <f>CONCATENATE(K3," DigiKey Part: ",H3," (",E3,")")</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -2065,7 +2080,7 @@
         <v>32</v>
       </c>
       <c r="L4" t="str">
-        <f>CONCATENATE(K4," DigiKey Part: ",H4," (",E4,")")</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -2104,7 +2119,7 @@
         <v>32</v>
       </c>
       <c r="L5" t="str">
-        <f>CONCATENATE(K5," DigiKey Part: ",H5," (",E5,")")</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -2143,7 +2158,7 @@
         <v>32</v>
       </c>
       <c r="L6" t="str">
-        <f>CONCATENATE(K6," DigiKey Part: ",H6," (",E6,")")</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -2182,7 +2197,7 @@
         <v>32</v>
       </c>
       <c r="L7" t="str">
-        <f>CONCATENATE(K7," DigiKey Part: ",H7," (",E7,")")</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -2221,7 +2236,7 @@
         <v>45</v>
       </c>
       <c r="L8" t="str">
-        <f>CONCATENATE(K8," DigiKey Part: ",H8," (",E8,")")</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -2260,7 +2275,7 @@
         <v>45</v>
       </c>
       <c r="L9" t="str">
-        <f>CONCATENATE(K9," DigiKey Part: ",H9," (",E9,")")</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -2299,7 +2314,7 @@
         <v>45</v>
       </c>
       <c r="L10" t="str">
-        <f>CONCATENATE(K10," DigiKey Part: ",H10," (",E10,")")</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -2338,7 +2353,7 @@
         <v>45</v>
       </c>
       <c r="L11" t="str">
-        <f>CONCATENATE(K11," DigiKey Part: ",H11," (",E11,")")</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -2377,7 +2392,7 @@
         <v>45</v>
       </c>
       <c r="L12" t="str">
-        <f>CONCATENATE(K12," DigiKey Part: ",H12," (",E12,")")</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -2416,7 +2431,7 @@
         <v>45</v>
       </c>
       <c r="L13" t="str">
-        <f>CONCATENATE(K13," DigiKey Part: ",H13," (",E13,")")</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -2455,7 +2470,7 @@
         <v>45</v>
       </c>
       <c r="L14" t="str">
-        <f>CONCATENATE(K14," DigiKey Part: ",H14," (",E14,")")</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10561-ND (1x2 power)</v>
       </c>
     </row>
@@ -2494,7 +2509,7 @@
         <v>44</v>
       </c>
       <c r="L15" t="str">
-        <f>CONCATENATE(K15," DigiKey Part: ",H15," (",E15,")")</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -2533,7 +2548,7 @@
         <v>44</v>
       </c>
       <c r="L16" t="str">
-        <f>CONCATENATE(K16," DigiKey Part: ",H16," (",E16,")")</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -2572,7 +2587,7 @@
         <v>44</v>
       </c>
       <c r="L17" t="str">
-        <f>CONCATENATE(K17," DigiKey Part: ",H17," (",E17,")")</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -2611,7 +2626,7 @@
         <v>44</v>
       </c>
       <c r="L18" t="str">
-        <f>CONCATENATE(K18," DigiKey Part: ",H18," (",E18,")")</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -2650,7 +2665,7 @@
         <v>44</v>
       </c>
       <c r="L19" t="str">
-        <f>CONCATENATE(K19," DigiKey Part: ",H19," (",E19,")")</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -2689,7 +2704,7 @@
         <v>44</v>
       </c>
       <c r="L20" t="str">
-        <f>CONCATENATE(K20," DigiKey Part: ",H20," (",E20,")")</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -2728,7 +2743,7 @@
         <v>35</v>
       </c>
       <c r="L21" t="str">
-        <f>CONCATENATE(K21," DigiKey Part: ",H21," (",E21,")")</f>
+        <f t="shared" si="0"/>
         <v>Serial Header DigiKey Part: 609-3263-ND (6x1 male)</v>
       </c>
     </row>
@@ -2767,7 +2782,7 @@
         <v>46</v>
       </c>
       <c r="L22" t="str">
-        <f>CONCATENATE(K22," DigiKey Part: ",H22," (",E22,")")</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -2806,7 +2821,7 @@
         <v>46</v>
       </c>
       <c r="L23" t="str">
-        <f>CONCATENATE(K23," DigiKey Part: ",H23," (",E23,")")</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -2845,7 +2860,7 @@
         <v>46</v>
       </c>
       <c r="L24" t="str">
-        <f>CONCATENATE(K24," DigiKey Part: ",H24," (",E24,")")</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -2884,7 +2899,7 @@
         <v>46</v>
       </c>
       <c r="L25" t="str">
-        <f>CONCATENATE(K25," DigiKey Part: ",H25," (",E25,")")</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -2923,7 +2938,7 @@
         <v>46</v>
       </c>
       <c r="L26" t="str">
-        <f>CONCATENATE(K26," DigiKey Part: ",H26," (",E26,")")</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -2962,7 +2977,7 @@
         <v>46</v>
       </c>
       <c r="L27" t="str">
-        <f>CONCATENATE(K27," DigiKey Part: ",H27," (",E27,")")</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -3001,7 +3016,7 @@
         <v>47</v>
       </c>
       <c r="L28" t="str">
-        <f>CONCATENATE(K28," DigiKey Part: ",H28," (",E28,")")</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -3040,7 +3055,7 @@
         <v>47</v>
       </c>
       <c r="L29" t="str">
-        <f>CONCATENATE(K29," DigiKey Part: ",H29," (",E29,")")</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -3079,7 +3094,7 @@
         <v>47</v>
       </c>
       <c r="L30" t="str">
-        <f>CONCATENATE(K30," DigiKey Part: ",H30," (",E30,")")</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -3118,7 +3133,7 @@
         <v>47</v>
       </c>
       <c r="L31" t="str">
-        <f>CONCATENATE(K31," DigiKey Part: ",H31," (",E31,")")</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -3157,7 +3172,7 @@
         <v>47</v>
       </c>
       <c r="L32" t="str">
-        <f>CONCATENATE(K32," DigiKey Part: ",H32," (",E32,")")</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -3196,7 +3211,7 @@
         <v>47</v>
       </c>
       <c r="L33" t="str">
-        <f>CONCATENATE(K33," DigiKey Part: ",H33," (",E33,")")</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -3681,10 +3696,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J15"/>
+  <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3698,7 +3713,7 @@
     <col min="9" max="9" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>76</v>
       </c>
@@ -3735,8 +3750,11 @@
         <f>CONCATENATE("Total (",D2,")")</f>
         <v>Total (12)</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="K1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>Pivot!A2</f>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
@@ -3752,12 +3770,12 @@
         <v>12</v>
       </c>
       <c r="E2">
-        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A2)*C2*1.1,1)</f>
-        <v>40</v>
+        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A2)*C2,1)</f>
+        <v>36</v>
       </c>
       <c r="F2">
-        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A2)*D2*1.1,1)</f>
-        <v>80</v>
+        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A2)*D2,1)</f>
+        <v>72</v>
       </c>
       <c r="G2" s="7">
         <f>GETPIVOTDATA(CONCATENATE("Sum of Price (",C2,")"),Pivot!$A$1,"Full Descruption",$A2)</f>
@@ -3768,21 +3786,24 @@
         <v>3.3000000000000002E-2</v>
       </c>
       <c r="I2">
-        <f>G2*E2</f>
-        <v>1.56</v>
+        <f t="shared" ref="I2:I12" si="0">G2*E2</f>
+        <v>1.4039999999999999</v>
       </c>
       <c r="J2">
-        <f>H2*F2</f>
-        <v>2.64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" ref="J2:J12" si="1">H2*F2</f>
+        <v>2.3760000000000003</v>
+      </c>
+      <c r="K2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
         <f>Pivot!A3</f>
         <v>Electrolitic Cap DigiKey Part: 732-9353-1-ND (10µF)</v>
       </c>
       <c r="B3" t="str">
-        <f t="shared" ref="B3:B12" si="0">TRIM(MID(A3,FIND(":",A3)+1,FIND("(",A3)-FIND(":",A3)-1))</f>
+        <f t="shared" ref="B3:B12" si="2">TRIM(MID(A3,FIND(":",A3)+1,FIND("(",A3)-FIND(":",A3)-1))</f>
         <v>732-9353-1-ND</v>
       </c>
       <c r="C3">
@@ -3808,21 +3829,21 @@
         <v>0.14499999999999999</v>
       </c>
       <c r="I3">
-        <f>G3*E3</f>
+        <f t="shared" si="0"/>
         <v>1.1900000000000002</v>
       </c>
       <c r="J3">
-        <f>H3*F3</f>
+        <f t="shared" si="1"/>
         <v>2.0299999999999998</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
         <f>Pivot!A4</f>
         <v>Header for BBB DigiKey Part: S2011EC-23-ND (23x2 Male Header)</v>
       </c>
       <c r="B4" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>S2011EC-23-ND</v>
       </c>
       <c r="C4">
@@ -3848,21 +3869,21 @@
         <v>0.91700000000000004</v>
       </c>
       <c r="I4">
-        <f>G4*E4</f>
+        <f t="shared" si="0"/>
         <v>12.838000000000001</v>
       </c>
       <c r="J4">
-        <f>H4*F4</f>
+        <f t="shared" si="1"/>
         <v>24.759</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>Pivot!A5</f>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
       <c r="B5" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>RHM1619CT-ND</v>
       </c>
       <c r="C5">
@@ -3872,12 +3893,12 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A5)*C5*1.1,1)</f>
-        <v>40</v>
+        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A5)*C5,1)</f>
+        <v>36</v>
       </c>
       <c r="F5">
-        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A5)*D5*1.1,1)</f>
-        <v>80</v>
+        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A5)*D5,1)</f>
+        <v>72</v>
       </c>
       <c r="G5" s="7">
         <f>GETPIVOTDATA(CONCATENATE("Sum of Price (",C5,")"),Pivot!$A$1,"Full Descruption",$A5)</f>
@@ -3888,21 +3909,24 @@
         <v>0.1268</v>
       </c>
       <c r="I5">
-        <f>G5*E5</f>
-        <v>5.0720000000000001</v>
+        <f t="shared" si="0"/>
+        <v>4.5648</v>
       </c>
       <c r="J5">
-        <f>H5*F5</f>
-        <v>10.144</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>9.1295999999999999</v>
+      </c>
+      <c r="K5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
         <f>Pivot!A6</f>
         <v>Serial Header DigiKey Part: 609-3263-ND (6x1 male)</v>
       </c>
       <c r="B6" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>609-3263-ND</v>
       </c>
       <c r="C6">
@@ -3928,21 +3952,21 @@
         <v>0.22500000000000001</v>
       </c>
       <c r="I6">
-        <f>G6*E6</f>
+        <f t="shared" si="0"/>
         <v>1.68</v>
       </c>
       <c r="J6">
-        <f>H6*F6</f>
+        <f t="shared" si="1"/>
         <v>3.15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
         <f>Pivot!A7</f>
         <v>Serial Header for BBB DigiKey Part: S7039-ND (6x1 female Header)</v>
       </c>
       <c r="B7" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>S7039-ND</v>
       </c>
       <c r="C7">
@@ -3968,21 +3992,21 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="I7">
-        <f>G7*E7</f>
+        <f t="shared" si="0"/>
         <v>4.8999999999999995</v>
       </c>
       <c r="J7">
-        <f>H7*F7</f>
+        <f t="shared" si="1"/>
         <v>7.6440000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
         <f>Pivot!A8</f>
         <v>Tac Switch DigiKey Part: 679-2428-ND (Switch)</v>
       </c>
       <c r="B8" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>679-2428-ND</v>
       </c>
       <c r="C8">
@@ -4008,21 +4032,21 @@
         <v>8.9599999999999999E-2</v>
       </c>
       <c r="I8">
-        <f>G8*E8</f>
+        <f t="shared" si="0"/>
         <v>1.302</v>
       </c>
       <c r="J8">
-        <f>H8*F8</f>
+        <f t="shared" si="1"/>
         <v>2.4192</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
         <f>Pivot!A9</f>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
       <c r="B9" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ED10566-ND</v>
       </c>
       <c r="C9">
@@ -4048,21 +4072,21 @@
         <v>1.7789999999999999</v>
       </c>
       <c r="I9">
-        <f>G9*E9</f>
+        <f t="shared" si="0"/>
         <v>78.400000000000006</v>
       </c>
       <c r="J9">
-        <f>H9*F9</f>
+        <f t="shared" si="1"/>
         <v>142.32</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
         <f>Pivot!A10</f>
         <v>Terminal Block DigiKey Part: ED10561-ND (1x2 power)</v>
       </c>
       <c r="B10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ED10561-ND</v>
       </c>
       <c r="C10">
@@ -4088,21 +4112,21 @@
         <v>0.54600000000000004</v>
       </c>
       <c r="I10">
-        <f>G10*E10</f>
+        <f t="shared" si="0"/>
         <v>4.0599999999999996</v>
       </c>
       <c r="J10">
-        <f>H10*F10</f>
+        <f t="shared" si="1"/>
         <v>7.6440000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
         <f>Pivot!A11</f>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
       <c r="B11" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>ED10523-ND</v>
       </c>
       <c r="C11">
@@ -4128,21 +4152,21 @@
         <v>0.27279999999999999</v>
       </c>
       <c r="I11">
-        <f>G11*E11</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="J11">
-        <f>H11*F11</f>
+        <f t="shared" si="1"/>
         <v>21.823999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>Pivot!A12</f>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
       <c r="B12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>296-13939-1-ND</v>
       </c>
       <c r="C12">
@@ -4152,12 +4176,12 @@
         <v>12</v>
       </c>
       <c r="E12">
-        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A12)*C12*1.1,1)</f>
-        <v>40</v>
+        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A12)*C12,1)</f>
+        <v>36</v>
       </c>
       <c r="F12">
-        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A12)*D12*1.1,1)</f>
-        <v>80</v>
+        <f>CEILING(GETPIVOTDATA("Sum of Quantity",Pivot!$A$1,"Full Descruption",Calc!$A12)*D12,1)</f>
+        <v>72</v>
       </c>
       <c r="G12" s="7">
         <f>GETPIVOTDATA(CONCATENATE("Sum of Price (",C12,")"),Pivot!$A$1,"Full Descruption",$A12)</f>
@@ -4168,35 +4192,73 @@
         <v>0.40600000000000003</v>
       </c>
       <c r="I12">
-        <f>G12*E12</f>
-        <v>16.240000000000002</v>
+        <f t="shared" si="0"/>
+        <v>14.616000000000001</v>
       </c>
       <c r="J12">
-        <f>H12*F12</f>
-        <v>32.480000000000004</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I14">
+        <f t="shared" si="1"/>
+        <v>29.232000000000003</v>
+      </c>
+      <c r="K12" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G13" s="7"/>
+      <c r="H13" s="7"/>
+    </row>
+    <row r="14" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="K14" t="s">
+        <v>87</v>
+      </c>
+      <c r="L14" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" s="9" customFormat="1" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="I15" s="9">
         <f>SUM(I2:I12)</f>
-        <v>142.24200000000002</v>
-      </c>
-      <c r="J14">
+        <v>139.95480000000001</v>
+      </c>
+      <c r="J15" s="9">
         <f>SUM(J2:J12)</f>
-        <v>257.05420000000004</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="I15">
-        <f>I14/C2</f>
-        <v>23.707000000000004</v>
-      </c>
-      <c r="J15">
-        <f>J14/D2</f>
-        <v>21.421183333333335</v>
+        <v>252.52779999999998</v>
+      </c>
+      <c r="K15" s="9">
+        <f>SUMIF($K2:$K12,"x",I2:I12)</f>
+        <v>20.584800000000001</v>
+      </c>
+      <c r="L15" s="9">
+        <f>SUMIF($K2:$K12,"x",J2:J12)</f>
+        <v>40.7376</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" s="8" customFormat="1" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="I16" s="8">
+        <f>I15/$C$2</f>
+        <v>23.325800000000001</v>
+      </c>
+      <c r="J16" s="8">
+        <f>J15/D2</f>
+        <v>21.043983333333333</v>
+      </c>
+      <c r="K16" s="8">
+        <f>K15/C2</f>
+        <v>3.4308000000000001</v>
+      </c>
+      <c r="L16" s="8">
+        <f>L15/D2</f>
+        <v>3.3948</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Latest iteration of the board with all the feedback incorporated. This is the version that was used for the PCBNG build. Also with the updated BOM for both SMT and through hole components
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,26 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="27795" windowHeight="13110" activeTab="2"/>
+    <workbookView xWindow="2640" yWindow="1935" windowWidth="27795" windowHeight="13110" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
     <sheet name="Pivot" sheetId="3" r:id="rId2"/>
     <sheet name="Calc" sheetId="5" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Calc!$A$1:$K$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet3!$A$1:$G$1</definedName>
     <definedName name="BOM">BOM!$A$1:$L$39</definedName>
+    <definedName name="PartNames">Sheet1!$A$2:$B$12</definedName>
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="3" r:id="rId4"/>
+    <pivotCache cacheId="6" r:id="rId6"/>
   </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="484" uniqueCount="146">
   <si>
     <t>#</t>
   </si>
@@ -304,6 +308,174 @@
   </si>
   <si>
     <t>Per Board</t>
+  </si>
+  <si>
+    <t>Digi-key-Part</t>
+  </si>
+  <si>
+    <t>RefDes</t>
+  </si>
+  <si>
+    <t>Mount</t>
+  </si>
+  <si>
+    <t>BBB1</t>
+  </si>
+  <si>
+    <t>BeagleBone-Black</t>
+  </si>
+  <si>
+    <t>BBB-P9-DIL-BOT</t>
+  </si>
+  <si>
+    <t>Through Hole</t>
+  </si>
+  <si>
+    <t>C1</t>
+  </si>
+  <si>
+    <t>.1uF</t>
+  </si>
+  <si>
+    <t>C2</t>
+  </si>
+  <si>
+    <t>C3</t>
+  </si>
+  <si>
+    <t>C4</t>
+  </si>
+  <si>
+    <t>C5</t>
+  </si>
+  <si>
+    <t>C6</t>
+  </si>
+  <si>
+    <t>J1</t>
+  </si>
+  <si>
+    <t>P0 - P7</t>
+  </si>
+  <si>
+    <t>J2</t>
+  </si>
+  <si>
+    <t>P8 - P15</t>
+  </si>
+  <si>
+    <t>J3</t>
+  </si>
+  <si>
+    <t>P16 - P23</t>
+  </si>
+  <si>
+    <t>J4</t>
+  </si>
+  <si>
+    <t>P24 - P31</t>
+  </si>
+  <si>
+    <t>J5</t>
+  </si>
+  <si>
+    <t>P32 - P39</t>
+  </si>
+  <si>
+    <t>J6</t>
+  </si>
+  <si>
+    <t>J7</t>
+  </si>
+  <si>
+    <t>5V 1amp</t>
+  </si>
+  <si>
+    <t>J13</t>
+  </si>
+  <si>
+    <t>J14</t>
+  </si>
+  <si>
+    <t>J15</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>J17</t>
+  </si>
+  <si>
+    <t>P32- P39</t>
+  </si>
+  <si>
+    <t>J18</t>
+  </si>
+  <si>
+    <t>P40 - P47</t>
+  </si>
+  <si>
+    <t>J19</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RHM1619CT-ND </t>
+  </si>
+  <si>
+    <t>100ohm</t>
+  </si>
+  <si>
+    <t>R2</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>R5</t>
+  </si>
+  <si>
+    <t>R6</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>U2</t>
+  </si>
+  <si>
+    <t>U3</t>
+  </si>
+  <si>
+    <t>U4</t>
+  </si>
+  <si>
+    <t>U5</t>
+  </si>
+  <si>
+    <t>U6</t>
+  </si>
+  <si>
+    <t>U7</t>
+  </si>
+  <si>
+    <t>U8</t>
+  </si>
+  <si>
+    <t>U9</t>
+  </si>
+  <si>
+    <t>10uF</t>
+  </si>
+  <si>
+    <t>BBB1-S</t>
+  </si>
+  <si>
+    <t>Description</t>
   </si>
 </sst>
 </file>
@@ -910,7 +1082,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Nick Rapoport" refreshedDate="42440.935864120373" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="38">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Nick Rapoport" refreshedDate="42442.05574895833" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="38">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:L39" sheet="BOM"/>
   </cacheSource>
@@ -1516,7 +1688,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -1911,8 +2083,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L39"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="E39" sqref="E39:H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3477,7 +3649,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:D2"/>
+      <pivotSelection pane="bottomRight" showHeader="1" extendable="1" axis="axisRow" max="12" activeRow="1" previousRow="1" click="1" r:id="rId1">
+        <pivotArea dataOnly="0" fieldPosition="0">
+          <references count="1">
+            <reference field="11" count="1">
+              <x v="0"/>
+            </reference>
+          </references>
+        </pivotArea>
+      </pivotSelection>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -3698,8 +3881,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4261,4 +4444,1060 @@
   <autoFilter ref="A1:K12"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="63.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>42</v>
+      </c>
+      <c r="B5" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>57</v>
+      </c>
+      <c r="B11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>58</v>
+      </c>
+      <c r="B12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState ref="A2:B12">
+    <sortCondition ref="A2:A12"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:L38"/>
+  <sheetViews>
+    <sheetView topLeftCell="B5" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="63.140625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="48.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G1" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>93</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D2" t="s">
+        <v>94</v>
+      </c>
+      <c r="E2" t="s">
+        <v>95</v>
+      </c>
+      <c r="F2" t="s">
+        <v>96</v>
+      </c>
+      <c r="G2" t="str">
+        <f>VLOOKUP(C2,PartNames,2)</f>
+        <v>Header for BBB DigiKey Part: S2011EC-23-ND (23x2 Male Header)</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F3" t="s">
+        <v>96</v>
+      </c>
+      <c r="G3" t="str">
+        <f>VLOOKUP(C3,PartNames,2)</f>
+        <v>Serial Header for BBB DigiKey Part: S7039-ND (6x1 female Header)</v>
+      </c>
+      <c r="L3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>97</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" t="s">
+        <v>98</v>
+      </c>
+      <c r="F4" t="s">
+        <v>86</v>
+      </c>
+      <c r="G4" t="str">
+        <f>VLOOKUP(C4,PartNames,2)</f>
+        <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" t="s">
+        <v>98</v>
+      </c>
+      <c r="F5" t="s">
+        <v>86</v>
+      </c>
+      <c r="G5" t="str">
+        <f>VLOOKUP(C5,PartNames,2)</f>
+        <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>100</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6" t="s">
+        <v>43</v>
+      </c>
+      <c r="D6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E6" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" t="s">
+        <v>86</v>
+      </c>
+      <c r="G6" t="str">
+        <f>VLOOKUP(C6,PartNames,2)</f>
+        <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>101</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="str">
+        <f>VLOOKUP(C7,PartNames,2)</f>
+        <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>98</v>
+      </c>
+      <c r="F8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G8" t="str">
+        <f>VLOOKUP(C8,PartNames,2)</f>
+        <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
+        <v>98</v>
+      </c>
+      <c r="F9" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" t="str">
+        <f>VLOOKUP(C9,PartNames,2)</f>
+        <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>38</v>
+      </c>
+      <c r="D10" t="s">
+        <v>9</v>
+      </c>
+      <c r="E10" t="s">
+        <v>105</v>
+      </c>
+      <c r="F10" t="s">
+        <v>96</v>
+      </c>
+      <c r="G10" t="str">
+        <f>VLOOKUP(C10,PartNames,2)</f>
+        <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>38</v>
+      </c>
+      <c r="D11" t="s">
+        <v>9</v>
+      </c>
+      <c r="E11" t="s">
+        <v>107</v>
+      </c>
+      <c r="F11" t="s">
+        <v>96</v>
+      </c>
+      <c r="G11" t="str">
+        <f>VLOOKUP(C11,PartNames,2)</f>
+        <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>108</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" t="s">
+        <v>9</v>
+      </c>
+      <c r="E12" t="s">
+        <v>109</v>
+      </c>
+      <c r="F12" t="s">
+        <v>96</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(C12,PartNames,2)</f>
+        <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>110</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" t="s">
+        <v>9</v>
+      </c>
+      <c r="E13" t="s">
+        <v>111</v>
+      </c>
+      <c r="F13" t="s">
+        <v>96</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(C13,PartNames,2)</f>
+        <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>112</v>
+      </c>
+      <c r="B14">
+        <v>1</v>
+      </c>
+      <c r="C14" t="s">
+        <v>38</v>
+      </c>
+      <c r="D14" t="s">
+        <v>9</v>
+      </c>
+      <c r="E14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14" t="s">
+        <v>96</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(C14,PartNames,2)</f>
+        <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>114</v>
+      </c>
+      <c r="B15">
+        <v>1</v>
+      </c>
+      <c r="C15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D15" t="s">
+        <v>9</v>
+      </c>
+      <c r="E15" t="s">
+        <v>105</v>
+      </c>
+      <c r="F15" t="s">
+        <v>96</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(C15,PartNames,2)</f>
+        <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+      <c r="D16" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" t="s">
+        <v>116</v>
+      </c>
+      <c r="F16" t="s">
+        <v>96</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(C16,PartNames,2)</f>
+        <v>Terminal Block DigiKey Part: ED10561-ND (1x2 power)</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>117</v>
+      </c>
+      <c r="B17">
+        <v>1</v>
+      </c>
+      <c r="C17" t="s">
+        <v>37</v>
+      </c>
+      <c r="D17" t="s">
+        <v>13</v>
+      </c>
+      <c r="E17" t="s">
+        <v>105</v>
+      </c>
+      <c r="F17" t="s">
+        <v>96</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(C17,PartNames,2)</f>
+        <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B18">
+        <v>1</v>
+      </c>
+      <c r="C18" t="s">
+        <v>37</v>
+      </c>
+      <c r="D18" t="s">
+        <v>13</v>
+      </c>
+      <c r="E18" t="s">
+        <v>107</v>
+      </c>
+      <c r="F18" t="s">
+        <v>96</v>
+      </c>
+      <c r="G18" t="str">
+        <f>VLOOKUP(C18,PartNames,2)</f>
+        <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>119</v>
+      </c>
+      <c r="B19">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>37</v>
+      </c>
+      <c r="D19" t="s">
+        <v>13</v>
+      </c>
+      <c r="E19" t="s">
+        <v>109</v>
+      </c>
+      <c r="F19" t="s">
+        <v>96</v>
+      </c>
+      <c r="G19" t="str">
+        <f>VLOOKUP(C19,PartNames,2)</f>
+        <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B20">
+        <v>1</v>
+      </c>
+      <c r="C20" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>111</v>
+      </c>
+      <c r="F20" t="s">
+        <v>96</v>
+      </c>
+      <c r="G20" t="str">
+        <f>VLOOKUP(C20,PartNames,2)</f>
+        <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>121</v>
+      </c>
+      <c r="B21">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>37</v>
+      </c>
+      <c r="D21" t="s">
+        <v>13</v>
+      </c>
+      <c r="E21" t="s">
+        <v>122</v>
+      </c>
+      <c r="F21" t="s">
+        <v>96</v>
+      </c>
+      <c r="G21" t="str">
+        <f>VLOOKUP(C21,PartNames,2)</f>
+        <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>123</v>
+      </c>
+      <c r="B22">
+        <v>1</v>
+      </c>
+      <c r="C22" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" t="s">
+        <v>13</v>
+      </c>
+      <c r="E22" t="s">
+        <v>124</v>
+      </c>
+      <c r="F22" t="s">
+        <v>96</v>
+      </c>
+      <c r="G22" t="str">
+        <f>VLOOKUP(C22,PartNames,2)</f>
+        <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>125</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>51</v>
+      </c>
+      <c r="D23" t="s">
+        <v>15</v>
+      </c>
+      <c r="E23" t="s">
+        <v>35</v>
+      </c>
+      <c r="F23" t="s">
+        <v>96</v>
+      </c>
+      <c r="G23" t="str">
+        <f>VLOOKUP(C23,PartNames,2)</f>
+        <v>Serial Header DigiKey Part: 609-3263-ND (6x1 male)</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>126</v>
+      </c>
+      <c r="B24">
+        <v>1</v>
+      </c>
+      <c r="C24" t="s">
+        <v>127</v>
+      </c>
+      <c r="D24" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" t="s">
+        <v>128</v>
+      </c>
+      <c r="F24" t="s">
+        <v>86</v>
+      </c>
+      <c r="G24" t="str">
+        <f>VLOOKUP(C24,PartNames,2)</f>
+        <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>129</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="C25" t="s">
+        <v>127</v>
+      </c>
+      <c r="D25" t="s">
+        <v>17</v>
+      </c>
+      <c r="E25" t="s">
+        <v>128</v>
+      </c>
+      <c r="F25" t="s">
+        <v>86</v>
+      </c>
+      <c r="G25" t="str">
+        <f>VLOOKUP(C25,PartNames,2)</f>
+        <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>130</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26" t="s">
+        <v>127</v>
+      </c>
+      <c r="D26" t="s">
+        <v>17</v>
+      </c>
+      <c r="E26" t="s">
+        <v>128</v>
+      </c>
+      <c r="F26" t="s">
+        <v>86</v>
+      </c>
+      <c r="G26" t="str">
+        <f>VLOOKUP(C26,PartNames,2)</f>
+        <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>131</v>
+      </c>
+      <c r="B27">
+        <v>1</v>
+      </c>
+      <c r="C27" t="s">
+        <v>127</v>
+      </c>
+      <c r="D27" t="s">
+        <v>17</v>
+      </c>
+      <c r="E27" t="s">
+        <v>128</v>
+      </c>
+      <c r="F27" t="s">
+        <v>86</v>
+      </c>
+      <c r="G27" t="str">
+        <f>VLOOKUP(C27,PartNames,2)</f>
+        <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>132</v>
+      </c>
+      <c r="B28">
+        <v>1</v>
+      </c>
+      <c r="C28" t="s">
+        <v>127</v>
+      </c>
+      <c r="D28" t="s">
+        <v>17</v>
+      </c>
+      <c r="E28" t="s">
+        <v>128</v>
+      </c>
+      <c r="F28" t="s">
+        <v>86</v>
+      </c>
+      <c r="G28" t="str">
+        <f>VLOOKUP(C28,PartNames,2)</f>
+        <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>133</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>127</v>
+      </c>
+      <c r="D29" t="s">
+        <v>17</v>
+      </c>
+      <c r="E29" t="s">
+        <v>128</v>
+      </c>
+      <c r="F29" t="s">
+        <v>86</v>
+      </c>
+      <c r="G29" t="str">
+        <f>VLOOKUP(C29,PartNames,2)</f>
+        <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>134</v>
+      </c>
+      <c r="B30">
+        <v>1</v>
+      </c>
+      <c r="C30" t="s">
+        <v>41</v>
+      </c>
+      <c r="D30" t="s">
+        <v>19</v>
+      </c>
+      <c r="E30" t="s">
+        <v>105</v>
+      </c>
+      <c r="F30" t="s">
+        <v>86</v>
+      </c>
+      <c r="G30" t="str">
+        <f>VLOOKUP(C30,PartNames,2)</f>
+        <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31" t="s">
+        <v>41</v>
+      </c>
+      <c r="D31" t="s">
+        <v>19</v>
+      </c>
+      <c r="E31" t="s">
+        <v>107</v>
+      </c>
+      <c r="F31" t="s">
+        <v>86</v>
+      </c>
+      <c r="G31" t="str">
+        <f>VLOOKUP(C31,PartNames,2)</f>
+        <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>136</v>
+      </c>
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D32" t="s">
+        <v>19</v>
+      </c>
+      <c r="E32" t="s">
+        <v>109</v>
+      </c>
+      <c r="F32" t="s">
+        <v>86</v>
+      </c>
+      <c r="G32" t="str">
+        <f>VLOOKUP(C32,PartNames,2)</f>
+        <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>137</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33" t="s">
+        <v>41</v>
+      </c>
+      <c r="D33" t="s">
+        <v>19</v>
+      </c>
+      <c r="E33" t="s">
+        <v>111</v>
+      </c>
+      <c r="F33" t="s">
+        <v>86</v>
+      </c>
+      <c r="G33" t="str">
+        <f>VLOOKUP(C33,PartNames,2)</f>
+        <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>138</v>
+      </c>
+      <c r="B34">
+        <v>1</v>
+      </c>
+      <c r="C34" t="s">
+        <v>41</v>
+      </c>
+      <c r="D34" t="s">
+        <v>19</v>
+      </c>
+      <c r="E34" t="s">
+        <v>113</v>
+      </c>
+      <c r="F34" t="s">
+        <v>86</v>
+      </c>
+      <c r="G34" t="str">
+        <f>VLOOKUP(C34,PartNames,2)</f>
+        <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>139</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="C35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D35" t="s">
+        <v>19</v>
+      </c>
+      <c r="E35" t="s">
+        <v>124</v>
+      </c>
+      <c r="F35" t="s">
+        <v>86</v>
+      </c>
+      <c r="G35" t="str">
+        <f>VLOOKUP(C35,PartNames,2)</f>
+        <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36" t="s">
+        <v>42</v>
+      </c>
+      <c r="D36" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" t="s">
+        <v>22</v>
+      </c>
+      <c r="F36" t="s">
+        <v>96</v>
+      </c>
+      <c r="G36" t="str">
+        <f>VLOOKUP(C36,PartNames,2)</f>
+        <v>Tac Switch DigiKey Part: 679-2428-ND (Switch)</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>141</v>
+      </c>
+      <c r="B37">
+        <v>1</v>
+      </c>
+      <c r="C37" t="s">
+        <v>42</v>
+      </c>
+      <c r="D37" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" t="s">
+        <v>96</v>
+      </c>
+      <c r="G37" t="str">
+        <f>VLOOKUP(C37,PartNames,2)</f>
+        <v>Tac Switch DigiKey Part: 679-2428-ND (Switch)</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>142</v>
+      </c>
+      <c r="B38">
+        <v>1</v>
+      </c>
+      <c r="C38" t="s">
+        <v>49</v>
+      </c>
+      <c r="D38" t="s">
+        <v>25</v>
+      </c>
+      <c r="E38" t="s">
+        <v>143</v>
+      </c>
+      <c r="F38" t="s">
+        <v>96</v>
+      </c>
+      <c r="G38" t="str">
+        <f>VLOOKUP(C38,PartNames,2)</f>
+        <v>Electrolitic Cap DigiKey Part: 732-9353-1-ND (10µF)</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:G1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Cleaned up the location of the silk screen.
</commit_message>
<xml_diff>
--- a/BOM.xlsx
+++ b/BOM.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="2640" yWindow="1935" windowWidth="27795" windowHeight="13110" activeTab="3"/>
+    <workbookView xWindow="2640" yWindow="1935" windowWidth="27795" windowHeight="13110" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,9 @@
   </definedNames>
   <calcPr calcId="145621"/>
   <pivotCaches>
-    <pivotCache cacheId="6" r:id="rId6"/>
+    <pivotCache cacheId="3" r:id="rId6"/>
   </pivotCaches>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -1082,7 +1083,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Nick Rapoport" refreshedDate="42442.05574895833" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="38">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Nick Rapoport" refreshedDate="42471.746017592595" createdVersion="4" refreshedVersion="4" minRefreshableVersion="3" recordCount="38">
   <cacheSource type="worksheet">
     <worksheetSource ref="A1:L39" sheet="BOM"/>
   </cacheSource>
@@ -1688,7 +1689,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="3" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="4" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="4" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="A1:D13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="12">
     <pivotField showAll="0"/>
@@ -3879,10 +3880,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr filterMode="1"/>
   <dimension ref="A1:L16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3937,7 +3939,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A2" t="str">
         <f>Pivot!A2</f>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
@@ -4060,7 +4062,7 @@
         <v>24.759</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
         <f>Pivot!A5</f>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
@@ -4343,7 +4345,7 @@
         <v>21.823999999999998</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" hidden="1" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
         <f>Pivot!A12</f>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
@@ -4441,7 +4443,11 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K12"/>
+  <autoFilter ref="A1:K12">
+    <filterColumn colId="10">
+      <filters blank="1"/>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4450,8 +4456,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4627,7 +4633,7 @@
         <v>96</v>
       </c>
       <c r="G2" t="str">
-        <f>VLOOKUP(C2,PartNames,2)</f>
+        <f t="shared" ref="G2:G38" si="0">VLOOKUP(C2,PartNames,2)</f>
         <v>Header for BBB DigiKey Part: S2011EC-23-ND (23x2 Male Header)</v>
       </c>
     </row>
@@ -4651,7 +4657,7 @@
         <v>96</v>
       </c>
       <c r="G3" t="str">
-        <f>VLOOKUP(C3,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Serial Header for BBB DigiKey Part: S7039-ND (6x1 female Header)</v>
       </c>
       <c r="L3" s="6"/>
@@ -4676,7 +4682,7 @@
         <v>86</v>
       </c>
       <c r="G4" t="str">
-        <f>VLOOKUP(C4,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -4700,7 +4706,7 @@
         <v>86</v>
       </c>
       <c r="G5" t="str">
-        <f>VLOOKUP(C5,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -4724,7 +4730,7 @@
         <v>86</v>
       </c>
       <c r="G6" t="str">
-        <f>VLOOKUP(C6,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -4748,7 +4754,7 @@
         <v>86</v>
       </c>
       <c r="G7" t="str">
-        <f>VLOOKUP(C7,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -4772,7 +4778,7 @@
         <v>86</v>
       </c>
       <c r="G8" t="str">
-        <f>VLOOKUP(C8,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -4796,7 +4802,7 @@
         <v>86</v>
       </c>
       <c r="G9" t="str">
-        <f>VLOOKUP(C9,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Ceramic Cap  DigiKey Part: 399-1249-1-ND (.1µF)</v>
       </c>
     </row>
@@ -4820,7 +4826,7 @@
         <v>96</v>
       </c>
       <c r="G10" t="str">
-        <f>VLOOKUP(C10,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -4844,7 +4850,7 @@
         <v>96</v>
       </c>
       <c r="G11" t="str">
-        <f>VLOOKUP(C11,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -4868,7 +4874,7 @@
         <v>96</v>
       </c>
       <c r="G12" t="str">
-        <f>VLOOKUP(C12,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -4892,7 +4898,7 @@
         <v>96</v>
       </c>
       <c r="G13" t="str">
-        <f>VLOOKUP(C13,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -4916,7 +4922,7 @@
         <v>96</v>
       </c>
       <c r="G14" t="str">
-        <f>VLOOKUP(C14,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -4940,7 +4946,7 @@
         <v>96</v>
       </c>
       <c r="G15" t="str">
-        <f>VLOOKUP(C15,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10566-ND (1x8 (Screw-down))</v>
       </c>
     </row>
@@ -4964,7 +4970,7 @@
         <v>96</v>
       </c>
       <c r="G16" t="str">
-        <f>VLOOKUP(C16,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Terminal Block DigiKey Part: ED10561-ND (1x2 power)</v>
       </c>
     </row>
@@ -4988,7 +4994,7 @@
         <v>96</v>
       </c>
       <c r="G17" t="str">
-        <f>VLOOKUP(C17,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -5012,7 +5018,7 @@
         <v>96</v>
       </c>
       <c r="G18" t="str">
-        <f>VLOOKUP(C18,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -5036,7 +5042,7 @@
         <v>96</v>
       </c>
       <c r="G19" t="str">
-        <f>VLOOKUP(C19,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -5060,7 +5066,7 @@
         <v>96</v>
       </c>
       <c r="G20" t="str">
-        <f>VLOOKUP(C20,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -5084,7 +5090,7 @@
         <v>96</v>
       </c>
       <c r="G21" t="str">
-        <f>VLOOKUP(C21,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -5108,7 +5114,7 @@
         <v>96</v>
       </c>
       <c r="G22" t="str">
-        <f>VLOOKUP(C22,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Shrouded Heder DigiKey Part: ED10523-ND (2x8 ribbon cable header)</v>
       </c>
     </row>
@@ -5132,7 +5138,7 @@
         <v>96</v>
       </c>
       <c r="G23" t="str">
-        <f>VLOOKUP(C23,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Serial Header DigiKey Part: 609-3263-ND (6x1 male)</v>
       </c>
     </row>
@@ -5156,7 +5162,7 @@
         <v>86</v>
       </c>
       <c r="G24" t="str">
-        <f>VLOOKUP(C24,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -5180,7 +5186,7 @@
         <v>86</v>
       </c>
       <c r="G25" t="str">
-        <f>VLOOKUP(C25,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -5204,7 +5210,7 @@
         <v>86</v>
       </c>
       <c r="G26" t="str">
-        <f>VLOOKUP(C26,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -5228,7 +5234,7 @@
         <v>86</v>
       </c>
       <c r="G27" t="str">
-        <f>VLOOKUP(C27,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -5252,7 +5258,7 @@
         <v>86</v>
       </c>
       <c r="G28" t="str">
-        <f>VLOOKUP(C28,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -5276,7 +5282,7 @@
         <v>86</v>
       </c>
       <c r="G29" t="str">
-        <f>VLOOKUP(C29,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Resistor Array DigiKey Part: RHM1619CT-ND (100Ω)</v>
       </c>
     </row>
@@ -5300,7 +5306,7 @@
         <v>86</v>
       </c>
       <c r="G30" t="str">
-        <f>VLOOKUP(C30,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -5324,7 +5330,7 @@
         <v>86</v>
       </c>
       <c r="G31" t="str">
-        <f>VLOOKUP(C31,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -5348,7 +5354,7 @@
         <v>86</v>
       </c>
       <c r="G32" t="str">
-        <f>VLOOKUP(C32,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -5372,7 +5378,7 @@
         <v>86</v>
       </c>
       <c r="G33" t="str">
-        <f>VLOOKUP(C33,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -5396,7 +5402,7 @@
         <v>86</v>
       </c>
       <c r="G34" t="str">
-        <f>VLOOKUP(C34,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -5420,7 +5426,7 @@
         <v>86</v>
       </c>
       <c r="G35" t="str">
-        <f>VLOOKUP(C35,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>TI Transceiver  DigiKey Part: 296-13939-1-ND (Transceiver )</v>
       </c>
     </row>
@@ -5444,7 +5450,7 @@
         <v>96</v>
       </c>
       <c r="G36" t="str">
-        <f>VLOOKUP(C36,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Tac Switch DigiKey Part: 679-2428-ND (Switch)</v>
       </c>
     </row>
@@ -5468,7 +5474,7 @@
         <v>96</v>
       </c>
       <c r="G37" t="str">
-        <f>VLOOKUP(C37,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Tac Switch DigiKey Part: 679-2428-ND (Switch)</v>
       </c>
     </row>
@@ -5492,7 +5498,7 @@
         <v>96</v>
       </c>
       <c r="G38" t="str">
-        <f>VLOOKUP(C38,PartNames,2)</f>
+        <f t="shared" si="0"/>
         <v>Electrolitic Cap DigiKey Part: 732-9353-1-ND (10µF)</v>
       </c>
     </row>

</xml_diff>